<commit_message>
Updated Landing Sales TP
</commit_message>
<xml_diff>
--- a/docs/tp/Sfera_4.0/TP NR LANDING SALES.xlsx
+++ b/docs/tp/Sfera_4.0/TP NR LANDING SALES.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\TA\matrix-web-fe-tests\docs\tp\Sfera_4.0\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F9EFA46-C3E2-4FD1-824A-42CA8E493181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441EBB28-4E67-4B12-BB21-5FF33C24EA00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8BA332EC-C50D-4B97-B356-D0AB195A852D}"/>
   </bookViews>
@@ -312,26 +312,26 @@
     <t>Allianz</t>
   </si>
   <si>
-    <t>DA FARE</t>
-  </si>
-  <si>
     <t>PRONTO GIA' IN RUN</t>
   </si>
   <si>
-    <t>PRONTO GIA' IN RUN (fare un check codice)</t>
-  </si>
-  <si>
     <t>PRONTO GIA' IN RUN (aggiungi verifica dati)</t>
   </si>
   <si>
     <t>Stato TA</t>
+  </si>
+  <si>
+    <t>FATTO</t>
+  </si>
+  <si>
+    <t>DA FARE ( PROBLEMA NESSUNA INIZIATIVA TROVATA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -344,8 +344,19 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -361,6 +372,24 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -392,7 +421,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -402,10 +431,37 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -725,15 +781,15 @@
   <dimension ref="A1:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D70" sqref="D70"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="40.7109375" customWidth="1"/>
     <col min="3" max="3" width="31.85546875" customWidth="1"/>
-    <col min="4" max="4" width="31.7109375" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
     <col min="5" max="5" width="13.28515625" customWidth="1"/>
     <col min="7" max="7" width="51.5703125" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
@@ -741,7 +797,7 @@
   <sheetData>
     <row r="1" spans="1:10" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>84</v>
@@ -773,7 +829,7 @@
     </row>
     <row r="2" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -833,7 +889,7 @@
     </row>
     <row r="5" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>9</v>
@@ -893,7 +949,7 @@
     </row>
     <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>13</v>
@@ -937,7 +993,7 @@
     </row>
     <row r="10" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>16</v>
@@ -979,97 +1035,97 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12" s="4" t="s">
+    <row r="12" spans="1:10" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A12" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B12" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
+      <c r="E12" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F12" s="3">
-        <v>2</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="F12" s="17">
+        <v>2</v>
+      </c>
+      <c r="G12" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="I12" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J12" s="17" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="4" t="s">
+    <row r="13" spans="1:10" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="D13" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-    </row>
-    <row r="14" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A14" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B14" s="4" t="s">
+      <c r="E13" s="17"/>
+      <c r="F13" s="17"/>
+      <c r="G13" s="17"/>
+      <c r="H13" s="17"/>
+      <c r="I13" s="17"/>
+      <c r="J13" s="17"/>
+    </row>
+    <row r="14" spans="1:10" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A14" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B14" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F14" s="3">
-        <v>2</v>
-      </c>
-      <c r="G14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="F14" s="17">
+        <v>2</v>
+      </c>
+      <c r="G14" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="I14" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J14" s="3" t="s">
+      <c r="J14" s="17" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="4" t="s">
+    <row r="15" spans="1:10" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="18" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="E15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
     </row>
     <row r="16" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>24</v>
@@ -1129,7 +1185,7 @@
     </row>
     <row r="19" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>29</v>
@@ -1171,837 +1227,837 @@
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
     </row>
-    <row r="21" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A21" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B21" s="4" t="s">
+    <row r="21" spans="1:10" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A21" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B21" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3" t="s">
+      <c r="C21" s="17"/>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F21" s="3">
-        <v>2</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21" s="3" t="s">
+      <c r="F21" s="17">
+        <v>2</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J21" s="3" t="s">
+      <c r="J21" s="17" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="4" t="s">
+    <row r="22" spans="1:10" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A22" s="17"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
-    </row>
-    <row r="23" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="4" t="s">
+      <c r="E22" s="17"/>
+      <c r="F22" s="17"/>
+      <c r="G22" s="17"/>
+      <c r="H22" s="17"/>
+      <c r="I22" s="17"/>
+      <c r="J22" s="17"/>
+    </row>
+    <row r="23" spans="1:10" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A23" s="17"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="D23" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
-      <c r="G23" s="3"/>
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
-      <c r="J23" s="3"/>
-    </row>
-    <row r="24" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A24" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B24" s="4" t="s">
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+    </row>
+    <row r="24" spans="1:10" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A24" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B24" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3" t="s">
+      <c r="C24" s="17"/>
+      <c r="D24" s="17"/>
+      <c r="E24" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F24" s="3">
-        <v>2</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H24" s="3" t="s">
+      <c r="F24" s="17">
+        <v>2</v>
+      </c>
+      <c r="G24" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J24" s="3" t="s">
+      <c r="J24" s="17" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="25" spans="1:10" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="4" t="s">
+    <row r="25" spans="1:10" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A25" s="17"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D25" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
-      <c r="J25" s="3"/>
-    </row>
-    <row r="26" spans="1:10" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="4" t="s">
+      <c r="E25" s="17"/>
+      <c r="F25" s="17"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="17"/>
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+    </row>
+    <row r="26" spans="1:10" s="19" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A26" s="17"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="D26" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
-    </row>
-    <row r="27" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="E26" s="17"/>
+      <c r="F26" s="17"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="17"/>
+      <c r="I26" s="17"/>
+      <c r="J26" s="17"/>
+    </row>
+    <row r="27" spans="1:10" s="7" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A27" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="F27" s="5">
+        <v>2</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" s="7" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A28" s="5"/>
+      <c r="B28" s="5"/>
+      <c r="C28" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5"/>
+    </row>
+    <row r="29" spans="1:10" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A29" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="B27" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3" t="s">
+      <c r="B29" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" s="17"/>
+      <c r="D29" s="17"/>
+      <c r="E29" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F27" s="3">
-        <v>2</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H27" s="3" t="s">
+      <c r="F29" s="17">
+        <v>2</v>
+      </c>
+      <c r="G29" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="I29" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J27" s="3" t="s">
+      <c r="J29" s="17" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-    </row>
-    <row r="29" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3" t="s">
+    <row r="30" spans="1:10" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A30" s="17"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="D30" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E30" s="17"/>
+      <c r="F30" s="17"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="17"/>
+      <c r="I30" s="17"/>
+      <c r="J30" s="17"/>
+    </row>
+    <row r="31" spans="1:10" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A31" s="17"/>
+      <c r="B31" s="17"/>
+      <c r="C31" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>48</v>
+      </c>
+      <c r="E31" s="17"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="17"/>
+      <c r="I31" s="17"/>
+      <c r="J31" s="17"/>
+    </row>
+    <row r="32" spans="1:10" s="19" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
+      <c r="A32" s="17"/>
+      <c r="B32" s="17"/>
+      <c r="C32" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D32" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="E32" s="17"/>
+      <c r="F32" s="17"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="17"/>
+      <c r="I32" s="17"/>
+      <c r="J32" s="17"/>
+    </row>
+    <row r="33" spans="1:10" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A33" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B33" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="17"/>
+      <c r="D33" s="17"/>
+      <c r="E33" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F29" s="3">
-        <v>2</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H29" s="3" t="s">
+      <c r="F33" s="17">
+        <v>2</v>
+      </c>
+      <c r="G33" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H33" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="I33" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J29" s="3" t="s">
+      <c r="J33" s="17" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="4" t="s">
+    <row r="34" spans="1:10" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A34" s="17"/>
+      <c r="B34" s="17"/>
+      <c r="C34" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D34" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-    </row>
-    <row r="31" spans="1:10" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="D31" s="3" t="s">
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+    </row>
+    <row r="35" spans="1:10" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A35" s="17"/>
+      <c r="B35" s="17"/>
+      <c r="C35" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D35" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-    </row>
-    <row r="32" spans="1:10" s="2" customFormat="1" ht="216.75" x14ac:dyDescent="0.2">
-      <c r="A32" s="3"/>
-      <c r="B32" s="3"/>
-      <c r="C32" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D32" s="3" t="s">
+      <c r="E35" s="17"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+    </row>
+    <row r="36" spans="1:10" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A36" s="17"/>
+      <c r="B36" s="17"/>
+      <c r="C36" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D36" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="3"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-    </row>
-    <row r="33" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A33" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B33" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3" t="s">
+      <c r="E36" s="17"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+    </row>
+    <row r="37" spans="1:10" s="19" customFormat="1" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C37" s="17"/>
+      <c r="D37" s="17"/>
+      <c r="E37" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F33" s="3">
-        <v>2</v>
-      </c>
-      <c r="G33" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H33" s="3" t="s">
+      <c r="F37" s="17">
+        <v>2</v>
+      </c>
+      <c r="G37" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H37" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="I37" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J33" s="3" t="s">
+      <c r="J37" s="17" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A34" s="3"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="4" t="s">
+    <row r="38" spans="1:10" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A38" s="17"/>
+      <c r="B38" s="17"/>
+      <c r="C38" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D38" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="3"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-    </row>
-    <row r="35" spans="1:10" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A35" s="3"/>
-      <c r="B35" s="3"/>
-      <c r="C35" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="D35" s="6" t="s">
+      <c r="E38" s="17"/>
+      <c r="F38" s="17"/>
+      <c r="G38" s="17"/>
+      <c r="H38" s="17"/>
+      <c r="I38" s="17"/>
+      <c r="J38" s="17"/>
+    </row>
+    <row r="39" spans="1:10" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A39" s="17"/>
+      <c r="B39" s="17"/>
+      <c r="C39" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="D39" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-      <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-    </row>
-    <row r="36" spans="1:10" s="2" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="4" t="s">
+      <c r="E39" s="17"/>
+      <c r="F39" s="17"/>
+      <c r="G39" s="17"/>
+      <c r="H39" s="17"/>
+      <c r="I39" s="17"/>
+      <c r="J39" s="17"/>
+    </row>
+    <row r="40" spans="1:10" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A40" s="17"/>
+      <c r="B40" s="17"/>
+      <c r="C40" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D36" s="6" t="s">
+      <c r="D40" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
-      <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-    </row>
-    <row r="37" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A37" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C37" s="3"/>
-      <c r="D37" s="3"/>
-      <c r="E37" s="3" t="s">
+      <c r="E40" s="17"/>
+      <c r="F40" s="17"/>
+      <c r="G40" s="17"/>
+      <c r="H40" s="17"/>
+      <c r="I40" s="17"/>
+      <c r="J40" s="17"/>
+    </row>
+    <row r="41" spans="1:10" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A41" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>56</v>
+      </c>
+      <c r="C41" s="17"/>
+      <c r="D41" s="17"/>
+      <c r="E41" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F37" s="3">
-        <v>2</v>
-      </c>
-      <c r="G37" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H37" s="3" t="s">
+      <c r="F41" s="17">
+        <v>2</v>
+      </c>
+      <c r="G41" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H41" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I37" s="3" t="s">
+      <c r="I41" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J37" s="3" t="s">
+      <c r="J41" s="17" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A38" s="3"/>
-      <c r="B38" s="3"/>
-      <c r="C38" s="4" t="s">
+    <row r="42" spans="1:10" s="19" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A42" s="17"/>
+      <c r="B42" s="17"/>
+      <c r="C42" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D42" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-    </row>
-    <row r="39" spans="1:10" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
-      <c r="B39" s="3"/>
-      <c r="C39" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="D39" s="6" t="s">
+      <c r="E42" s="17"/>
+      <c r="F42" s="17"/>
+      <c r="G42" s="17"/>
+      <c r="H42" s="17"/>
+      <c r="I42" s="17"/>
+      <c r="J42" s="17"/>
+    </row>
+    <row r="43" spans="1:10" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A43" s="17"/>
+      <c r="B43" s="17"/>
+      <c r="C43" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="D43" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="3"/>
-      <c r="H39" s="3"/>
-      <c r="I39" s="3"/>
-      <c r="J39" s="3"/>
-    </row>
-    <row r="40" spans="1:10" s="2" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="4" t="s">
+      <c r="E43" s="17"/>
+      <c r="F43" s="17"/>
+      <c r="G43" s="17"/>
+      <c r="H43" s="17"/>
+      <c r="I43" s="17"/>
+      <c r="J43" s="17"/>
+    </row>
+    <row r="44" spans="1:10" s="19" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
+      <c r="A44" s="17"/>
+      <c r="B44" s="17"/>
+      <c r="C44" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="D40" s="6" t="s">
+      <c r="D44" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E40" s="3"/>
-      <c r="F40" s="3"/>
-      <c r="G40" s="3"/>
-      <c r="H40" s="3"/>
-      <c r="I40" s="3"/>
-      <c r="J40" s="3"/>
-    </row>
-    <row r="41" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A41" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C41" s="3"/>
-      <c r="D41" s="3"/>
-      <c r="E41" s="3" t="s">
+      <c r="E44" s="17"/>
+      <c r="F44" s="17"/>
+      <c r="G44" s="17"/>
+      <c r="H44" s="17"/>
+      <c r="I44" s="17"/>
+      <c r="J44" s="17"/>
+    </row>
+    <row r="45" spans="1:10" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A45" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B45" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C45" s="17"/>
+      <c r="D45" s="17"/>
+      <c r="E45" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F41" s="3">
-        <v>2</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H41" s="3" t="s">
+      <c r="F45" s="17">
+        <v>2</v>
+      </c>
+      <c r="G45" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H45" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="I41" s="3" t="s">
+      <c r="I45" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="J41" s="3" t="s">
+      <c r="J45" s="17" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A42" s="3"/>
-      <c r="B42" s="3"/>
-      <c r="C42" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D42" s="3" t="s">
+    <row r="46" spans="1:10" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A46" s="17"/>
+      <c r="B46" s="17"/>
+      <c r="C46" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="D46" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E46" s="17"/>
+      <c r="F46" s="17"/>
+      <c r="G46" s="17"/>
+      <c r="H46" s="17"/>
+      <c r="I46" s="17"/>
+      <c r="J46" s="17"/>
+    </row>
+    <row r="47" spans="1:10" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A47" s="17"/>
+      <c r="B47" s="17"/>
+      <c r="C47" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D47" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="E47" s="17"/>
+      <c r="F47" s="17"/>
+      <c r="G47" s="17"/>
+      <c r="H47" s="17"/>
+      <c r="I47" s="17"/>
+      <c r="J47" s="17"/>
+    </row>
+    <row r="48" spans="1:10" s="19" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A48" s="17" t="s">
+        <v>97</v>
+      </c>
+      <c r="B48" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="C48" s="17"/>
+      <c r="D48" s="17"/>
+      <c r="E48" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="F48" s="17">
+        <v>2</v>
+      </c>
+      <c r="G48" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H48" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="I48" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="J48" s="17" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" s="19" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A49" s="17"/>
+      <c r="B49" s="17"/>
+      <c r="C49" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="D49" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E49" s="17"/>
+      <c r="F49" s="17"/>
+      <c r="G49" s="17"/>
+      <c r="H49" s="17"/>
+      <c r="I49" s="17"/>
+      <c r="J49" s="17"/>
+    </row>
+    <row r="50" spans="1:10" s="19" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
+      <c r="A50" s="17"/>
+      <c r="B50" s="17"/>
+      <c r="C50" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="D50" s="20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E50" s="17"/>
+      <c r="F50" s="17"/>
+      <c r="G50" s="17"/>
+      <c r="H50" s="17"/>
+      <c r="I50" s="17"/>
+      <c r="J50" s="17"/>
+    </row>
+    <row r="51" spans="1:10" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A51" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C51" s="8"/>
+      <c r="D51" s="8"/>
+      <c r="E51" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="F51" s="8">
+        <v>2</v>
+      </c>
+      <c r="G51" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H51" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="J51" s="8" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A52" s="8"/>
+      <c r="B52" s="8"/>
+      <c r="C52" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D52" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="E52" s="8"/>
+      <c r="F52" s="8"/>
+      <c r="G52" s="8"/>
+      <c r="H52" s="8"/>
+      <c r="I52" s="8"/>
+      <c r="J52" s="8"/>
+    </row>
+    <row r="53" spans="1:10" s="10" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A53" s="8"/>
+      <c r="B53" s="8"/>
+      <c r="C53" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="D53" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="E53" s="8"/>
+      <c r="F53" s="8"/>
+      <c r="G53" s="8"/>
+      <c r="H53" s="8"/>
+      <c r="I53" s="8"/>
+      <c r="J53" s="8"/>
+    </row>
+    <row r="54" spans="1:10" s="10" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A54" s="8"/>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="E54" s="8"/>
+      <c r="F54" s="8"/>
+      <c r="G54" s="8"/>
+      <c r="H54" s="8"/>
+      <c r="I54" s="8"/>
+      <c r="J54" s="8"/>
+    </row>
+    <row r="55" spans="1:10" s="10" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A55" s="8"/>
+      <c r="B55" s="8"/>
+      <c r="C55" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="E55" s="8"/>
+      <c r="F55" s="8"/>
+      <c r="G55" s="8"/>
+      <c r="H55" s="8"/>
+      <c r="I55" s="8"/>
+      <c r="J55" s="8"/>
+    </row>
+    <row r="56" spans="1:10" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A56" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B56" s="13" t="s">
+        <v>75</v>
+      </c>
+      <c r="C56" s="12"/>
+      <c r="D56" s="12"/>
+      <c r="E56" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F56" s="12">
+        <v>2</v>
+      </c>
+      <c r="G56" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H56" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I56" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J56" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
+      <c r="C57" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E57" s="12"/>
+      <c r="F57" s="12"/>
+      <c r="G57" s="12"/>
+      <c r="H57" s="12"/>
+      <c r="I57" s="12"/>
+      <c r="J57" s="12"/>
+    </row>
+    <row r="58" spans="1:10" s="14" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A58" s="15"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D58" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="E58" s="12"/>
+      <c r="F58" s="12"/>
+      <c r="G58" s="12"/>
+      <c r="H58" s="12"/>
+      <c r="I58" s="12"/>
+      <c r="J58" s="12"/>
+    </row>
+    <row r="59" spans="1:10" s="14" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="A59" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="B59" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C59" s="12"/>
+      <c r="D59" s="12"/>
+      <c r="E59" s="12" t="s">
+        <v>1</v>
+      </c>
+      <c r="F59" s="12">
+        <v>2</v>
+      </c>
+      <c r="G59" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H59" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="I59" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J59" s="12" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A60" s="12"/>
+      <c r="B60" s="12"/>
+      <c r="C60" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="D60" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="E60" s="12"/>
+      <c r="F60" s="12"/>
+      <c r="G60" s="12"/>
+      <c r="H60" s="12"/>
+      <c r="I60" s="12"/>
+      <c r="J60" s="12"/>
+    </row>
+    <row r="61" spans="1:10" s="14" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
+      <c r="C61" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D61" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E61" s="12"/>
+      <c r="F61" s="12"/>
+      <c r="G61" s="12"/>
+      <c r="H61" s="12"/>
+      <c r="I61" s="12"/>
+      <c r="J61" s="12"/>
+    </row>
+    <row r="62" spans="1:10" s="14" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="12"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D62" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-      <c r="G42" s="3"/>
-      <c r="H42" s="3"/>
-      <c r="I42" s="3"/>
-      <c r="J42" s="3"/>
-    </row>
-    <row r="43" spans="1:10" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-    </row>
-    <row r="44" spans="1:10" s="2" customFormat="1" ht="114.75" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-    </row>
-    <row r="45" spans="1:10" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A45" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F45" s="3">
-        <v>2</v>
-      </c>
-      <c r="G45" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H45" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I45" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J45" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-      <c r="B46" s="3"/>
-      <c r="C46" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E46" s="3"/>
-      <c r="F46" s="3"/>
-      <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
-      <c r="J46" s="3"/>
-    </row>
-    <row r="47" spans="1:10" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-      <c r="B47" s="3"/>
-      <c r="C47" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="E47" s="3"/>
-      <c r="F47" s="3"/>
-      <c r="G47" s="3"/>
-      <c r="H47" s="3"/>
-      <c r="I47" s="3"/>
-      <c r="J47" s="3"/>
-    </row>
-    <row r="48" spans="1:10" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A48" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C48" s="3"/>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F48" s="3">
-        <v>2</v>
-      </c>
-      <c r="G48" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H48" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I48" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J48" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D49" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-    </row>
-    <row r="50" spans="1:10" s="2" customFormat="1" ht="63.75" x14ac:dyDescent="0.2">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-      <c r="C50" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="3"/>
-      <c r="H50" s="3"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-    </row>
-    <row r="51" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A51" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C51" s="3"/>
-      <c r="D51" s="3"/>
-      <c r="E51" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F51" s="3">
-        <v>2</v>
-      </c>
-      <c r="G51" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H51" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I51" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J51" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-      <c r="C52" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D52" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-    </row>
-    <row r="53" spans="1:10" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3"/>
-      <c r="C53" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-    </row>
-    <row r="54" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A54" s="3"/>
-      <c r="B54" s="3"/>
-      <c r="C54" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="D54" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E54" s="3"/>
-      <c r="F54" s="3"/>
-      <c r="G54" s="3"/>
-      <c r="H54" s="3"/>
-      <c r="I54" s="3"/>
-      <c r="J54" s="3"/>
-    </row>
-    <row r="55" spans="1:10" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A55" s="3"/>
-      <c r="B55" s="3"/>
-      <c r="C55" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="D55" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
-      <c r="G55" s="3"/>
-      <c r="H55" s="3"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-    </row>
-    <row r="56" spans="1:10" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A56" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F56" s="3">
-        <v>2</v>
-      </c>
-      <c r="G56" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H56" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I56" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J56" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-      <c r="C57" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D57" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="E57" s="3"/>
-      <c r="F57" s="3"/>
-      <c r="G57" s="3"/>
-      <c r="H57" s="3"/>
-      <c r="I57" s="3"/>
-      <c r="J57" s="3"/>
-    </row>
-    <row r="58" spans="1:10" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A58" s="3"/>
-      <c r="B58" s="3"/>
-      <c r="C58" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="3"/>
-      <c r="J58" s="3"/>
-    </row>
-    <row r="59" spans="1:10" s="2" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A59" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>78</v>
-      </c>
-      <c r="C59" s="3"/>
-      <c r="D59" s="3"/>
-      <c r="E59" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="F59" s="3">
-        <v>2</v>
-      </c>
-      <c r="G59" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H59" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="I59" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J59" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-      <c r="C60" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="D60" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E60" s="3"/>
-      <c r="F60" s="3"/>
-      <c r="G60" s="3"/>
-      <c r="H60" s="3"/>
-      <c r="I60" s="3"/>
-      <c r="J60" s="3"/>
-    </row>
-    <row r="61" spans="1:10" s="2" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-      <c r="C61" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="D61" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="3"/>
-    </row>
-    <row r="62" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
-    </row>
-    <row r="63" spans="1:10" s="2" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-      <c r="C63" s="4" t="s">
+      <c r="E62" s="12"/>
+      <c r="F62" s="12"/>
+      <c r="G62" s="12"/>
+      <c r="H62" s="12"/>
+      <c r="I62" s="12"/>
+      <c r="J62" s="12"/>
+    </row>
+    <row r="63" spans="1:10" s="14" customFormat="1" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A63" s="12"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="D63" s="3" t="s">
+      <c r="D63" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="3"/>
-      <c r="J63" s="3"/>
+      <c r="E63" s="12"/>
+      <c r="F63" s="12"/>
+      <c r="G63" s="12"/>
+      <c r="H63" s="12"/>
+      <c r="I63" s="12"/>
+      <c r="J63" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J63" xr:uid="{65045D10-FA97-46ED-B50C-234823C9DE90}"/>

</xml_diff>